<commit_message>
old computer: final commit
</commit_message>
<xml_diff>
--- a/KETEK/dV_dT.xlsx
+++ b/KETEK/dV_dT.xlsx
@@ -939,11 +939,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="30571520"/>
-        <c:axId val="30585600"/>
+        <c:axId val="76389376"/>
+        <c:axId val="76399360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30571520"/>
+        <c:axId val="76389376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -953,12 +953,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30585600"/>
+        <c:crossAx val="76399360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30585600"/>
+        <c:axId val="76399360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1050"/>
@@ -971,7 +971,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30571520"/>
+        <c:crossAx val="76389376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1111,11 +1111,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="30503680"/>
-        <c:axId val="30505216"/>
+        <c:axId val="76571392"/>
+        <c:axId val="76572928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30503680"/>
+        <c:axId val="76571392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,12 +1125,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30505216"/>
+        <c:crossAx val="76572928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30505216"/>
+        <c:axId val="76572928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,7 +1141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30503680"/>
+        <c:crossAx val="76571392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1443,11 +1443,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="30891008"/>
-        <c:axId val="30892800"/>
+        <c:axId val="76508160"/>
+        <c:axId val="76509952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30891008"/>
+        <c:axId val="76508160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,12 +1457,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30892800"/>
+        <c:crossAx val="76509952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30892800"/>
+        <c:axId val="76509952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1475,7 +1475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30891008"/>
+        <c:crossAx val="76508160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1603,11 +1603,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="30913664"/>
-        <c:axId val="30915200"/>
+        <c:axId val="76530816"/>
+        <c:axId val="76532352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30913664"/>
+        <c:axId val="76530816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,12 +1617,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30915200"/>
+        <c:crossAx val="76532352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30915200"/>
+        <c:axId val="76532352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1633,7 +1633,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30913664"/>
+        <c:crossAx val="76530816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1755,11 +1755,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72562176"/>
-        <c:axId val="72560640"/>
+        <c:axId val="76915840"/>
+        <c:axId val="76917376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72562176"/>
+        <c:axId val="76915840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,12 +1769,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72560640"/>
+        <c:crossAx val="76917376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72560640"/>
+        <c:axId val="76917376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1785,7 +1785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72562176"/>
+        <c:crossAx val="76915840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1901,11 +1901,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72931200"/>
-        <c:axId val="72929664"/>
+        <c:axId val="77901184"/>
+        <c:axId val="77907072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72931200"/>
+        <c:axId val="77901184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1915,12 +1915,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72929664"/>
+        <c:crossAx val="77907072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72929664"/>
+        <c:axId val="77907072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1931,7 +1931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72931200"/>
+        <c:crossAx val="77901184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2047,11 +2047,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="30858624"/>
-        <c:axId val="30864512"/>
+        <c:axId val="77930880"/>
+        <c:axId val="77932416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30858624"/>
+        <c:axId val="77930880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2061,12 +2061,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30864512"/>
+        <c:crossAx val="77932416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30864512"/>
+        <c:axId val="77932416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2077,7 +2077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30858624"/>
+        <c:crossAx val="77930880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6110,7 +6110,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>